<commit_message>
adicao de varias coisas e modificacao de varias outras mas nao deu certo muitas coisas, ent tudo ira mudar novamente depois
</commit_message>
<xml_diff>
--- a/data/dim_person_master.xlsx
+++ b/data/dim_person_master.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06D7EA72-A513-4948-B8F9-CE8A82C7564C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21A75DB6-91E0-4D79-AE06-FDDBAA0C596F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro_Mestre" sheetId="1" r:id="rId1"/>
     <sheet name="Times" sheetId="2" r:id="rId2"/>
+    <sheet name="Campeonatos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="108">
   <si>
     <t>Nome</t>
   </si>
@@ -92,6 +93,21 @@
     <t>880.953.950-80</t>
   </si>
   <si>
+    <t>Beatriz Lima</t>
+  </si>
+  <si>
+    <t>570.661.030-41</t>
+  </si>
+  <si>
+    <t>Ex - Atleta</t>
+  </si>
+  <si>
+    <t>Beatriz Waricoda</t>
+  </si>
+  <si>
+    <t>876.941.320-78</t>
+  </si>
+  <si>
     <t>Bruna Kiyono</t>
   </si>
   <si>
@@ -122,18 +138,18 @@
     <t>152.503.150-38</t>
   </si>
   <si>
+    <t>Gabriel de Oliveira</t>
+  </si>
+  <si>
+    <t>341.251.760-78</t>
+  </si>
+  <si>
     <t>Gabriel Trigolo</t>
   </si>
   <si>
     <t>790.068.370-40</t>
   </si>
   <si>
-    <t>Gabriel de Oliveira</t>
-  </si>
-  <si>
-    <t>341.251.760-78</t>
-  </si>
-  <si>
     <t>Gustavo Ribeiro</t>
   </si>
   <si>
@@ -194,6 +210,12 @@
     <t>711.031.530-48</t>
   </si>
   <si>
+    <t>Leonardo Rocha</t>
+  </si>
+  <si>
+    <t>030.535.760-31</t>
+  </si>
+  <si>
     <t>Letícia Pereira</t>
   </si>
   <si>
@@ -242,15 +264,21 @@
     <t>595.025.730-80</t>
   </si>
   <si>
-    <t>Ex - Atleta</t>
-  </si>
-  <si>
     <t>Mateus Pazinatto</t>
   </si>
   <si>
     <t>451.727.610-47</t>
   </si>
   <si>
+    <t>Matheus Durão</t>
+  </si>
+  <si>
+    <t>067.960.780-39</t>
+  </si>
+  <si>
+    <t>Associado</t>
+  </si>
+  <si>
     <t>Matheus Fenili</t>
   </si>
   <si>
@@ -269,6 +297,12 @@
     <t>504.682.600-30</t>
   </si>
   <si>
+    <t>Pedro Oliveira</t>
+  </si>
+  <si>
+    <t>145.806.020-99</t>
+  </si>
+  <si>
     <t>Rhafaela  Oliveira</t>
   </si>
   <si>
@@ -281,65 +315,80 @@
     <t>591.381.000-70</t>
   </si>
   <si>
-    <t>Beatriz Lima</t>
-  </si>
-  <si>
-    <t>570.661.030-41</t>
-  </si>
-  <si>
-    <t>Leonardo Rocha</t>
-  </si>
-  <si>
-    <t>030.535.760-31</t>
-  </si>
-  <si>
-    <t>Matheus Durão</t>
-  </si>
-  <si>
-    <t>067.960.780-39</t>
-  </si>
-  <si>
-    <t>Associado</t>
-  </si>
-  <si>
-    <t>Pedro Oliveira</t>
-  </si>
-  <si>
-    <t>145.806.020-99</t>
-  </si>
-  <si>
-    <t>Beatriz Waricoda</t>
-  </si>
-  <si>
-    <t>876.941.320-78</t>
-  </si>
-  <si>
-    <t>Times Principais</t>
-  </si>
-  <si>
-    <t>Times Extras</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
+    <t>Tipo - Time</t>
+  </si>
+  <si>
     <t>C2 - Phoenix</t>
   </si>
   <si>
+    <t>Principal - COED</t>
+  </si>
+  <si>
+    <t>C3 - Immortals</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>AS C2 - Betas</t>
   </si>
   <si>
-    <t>C3 - Immortals</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Extra - Stunt</t>
+  </si>
+  <si>
+    <t>Nome_Time</t>
+  </si>
+  <si>
+    <t>Nome_Campeonato</t>
+  </si>
+  <si>
+    <t>Modalidade</t>
+  </si>
+  <si>
+    <t>Custo_Atleta</t>
+  </si>
+  <si>
+    <t>Pontuação Final</t>
+  </si>
+  <si>
+    <t>Colocação</t>
+  </si>
+  <si>
+    <t>Times Cadastrados</t>
+  </si>
+  <si>
+    <t>Betas</t>
+  </si>
+  <si>
+    <t>Arena - 2026</t>
+  </si>
+  <si>
+    <t>Group Stunt</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Cheerfest - 2025</t>
+  </si>
+  <si>
+    <t>Team Cheer</t>
+  </si>
+  <si>
+    <t>Immortals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +416,14 @@
       <name val="Aptos Narrow"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -377,18 +434,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.749992370372631"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -396,31 +453,276 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -456,14 +758,45 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15B5352D-8AD5-47AA-8875-8B00ECA83E91}" name="Tabela1" displayName="Tabela1" ref="A1:E70" totalsRowShown="0">
   <autoFilter ref="A1:E70" xr:uid="{15B5352D-8AD5-47AA-8875-8B00ECA83E91}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E70">
+    <sortCondition ref="A1:A70"/>
+  </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{30EAB156-D5F2-46F8-9E8F-B9F613F56D75}" name="Nome" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{30EAB156-D5F2-46F8-9E8F-B9F613F56D75}" name="Nome" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{C491A658-9F0B-4089-9148-88B0DE4B40C5}" name="CPF"/>
     <tableColumn id="3" xr3:uid="{3D238B38-666C-40A5-8487-A5606FEBA449}" name="Categoria"/>
     <tableColumn id="4" xr3:uid="{EB4FD1F2-5CB2-45F6-9B5D-17DC0ADE4AF7}" name="Entrada-Time"/>
     <tableColumn id="5" xr3:uid="{971FF1D4-6850-4942-942F-5099DE9342BA}" name="Saida-Time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{683CA54B-9E7A-463A-BA14-94DE8B1B0C56}" name="Tabela3" displayName="Tabela3" ref="A1:D39" totalsRowShown="0">
+  <autoFilter ref="A1:D39" xr:uid="{683CA54B-9E7A-463A-BA14-94DE8B1B0C56}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{840379C5-E585-4DD4-A703-EB61A64A5BD9}" name="Nome"/>
+    <tableColumn id="2" xr3:uid="{F9B2F450-D1CC-4E74-AE78-FCA01C3F86AB}" name="CPF"/>
+    <tableColumn id="3" xr3:uid="{29F084AA-C0DC-4301-8672-AC4F6D7ED3FA}" name="Time"/>
+    <tableColumn id="4" xr3:uid="{F45E8286-79FC-4550-A96C-C40BDABC8AB1}" name="Tipo - Time"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{599304BD-009D-4E9A-BCDC-6482628B4A90}" name="Tabela5" displayName="Tabela5" ref="A1:F4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A1:F4" xr:uid="{599304BD-009D-4E9A-BCDC-6482628B4A90}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{F3C79F78-6277-486C-A311-394F5A0DD12D}" name="Nome_Time" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4F465161-10F0-43C3-BFF7-7FA47BF7171B}" name="Nome_Campeonato" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E115701B-1B40-476B-92AB-892EBA616270}" name="Modalidade" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{5585512A-0AB3-4D30-AC79-FD962D46779F}" name="Custo_Atleta" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{BDB7ACC7-72D5-4B06-A466-C822C2F7A161}" name="Pontuação Final" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{861E06DF-761C-4779-8F23-D15A6047A740}" name="Colocação" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -786,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -826,10 +1159,10 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>45717</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="18">
       <c r="A3" s="2" t="s">
@@ -841,7 +1174,7 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>45717</v>
       </c>
     </row>
@@ -855,77 +1188,83 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>45505</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18">
-      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="4">
+        <v>45658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5">
-        <v>45505</v>
+        <v>14</v>
+      </c>
+      <c r="E6" s="4">
+        <v>45658</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
-      </c>
-      <c r="D7" s="5">
-        <v>45505</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>45505</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45505</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -933,10 +1272,10 @@
     </row>
     <row r="11" spans="1:5" ht="18">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -944,77 +1283,74 @@
     </row>
     <row r="12" spans="1:5" ht="18">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
-      </c>
-      <c r="D12" s="5">
-        <v>45717</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
-      </c>
-      <c r="D13" s="5">
-        <v>45717</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>45717</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
+      </c>
+      <c r="D15" s="4">
+        <v>45717</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>45717</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1022,60 +1358,63 @@
     </row>
     <row r="18" spans="1:5" ht="18">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>45717</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
-      </c>
-      <c r="D19" s="5">
-        <v>45717</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45717</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45717</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1083,97 +1422,88 @@
     </row>
     <row r="23" spans="1:5" ht="18">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18">
-      <c r="A24" s="2" t="s">
-        <v>50</v>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45658</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
-      </c>
-      <c r="D25" s="5">
-        <v>45505</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
-      </c>
-      <c r="D26" s="5">
-        <v>45717</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
-      </c>
-      <c r="D27" s="5">
-        <v>45505</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="5">
-        <v>45717</v>
+      <c r="D28" s="4">
+        <v>45505</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="5">
-        <v>45505</v>
-      </c>
-      <c r="E29" s="5">
-        <v>45658</v>
+        <v>7</v>
+      </c>
+      <c r="D29" s="4">
+        <v>45717</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18">
@@ -1186,8 +1516,8 @@
       <c r="C30" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="5">
-        <v>45717</v>
+      <c r="D30" s="4">
+        <v>45505</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18">
@@ -1200,7 +1530,7 @@
       <c r="C31" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <v>45717</v>
       </c>
     </row>
@@ -1212,7 +1542,13 @@
         <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="D32" s="4">
+        <v>45505</v>
+      </c>
+      <c r="E32" s="4">
+        <v>45658</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18">
@@ -1225,103 +1561,100 @@
       <c r="C33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="18">
-      <c r="A34" s="2" t="s">
+      <c r="D33" s="4">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="5">
-        <v>45717</v>
+        <v>73</v>
+      </c>
+      <c r="E34" s="4">
+        <v>45658</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18">
       <c r="A35" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <v>45717</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="3" t="s">
-        <v>75</v>
+    <row r="36" spans="1:5" ht="18">
+      <c r="A36" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" s="5">
-        <v>45658</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="3" t="s">
-        <v>77</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="18">
+      <c r="A37" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="5">
-        <v>45658</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="5">
+        <v>73</v>
+      </c>
+      <c r="E38" s="4">
         <v>45658</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:5" ht="18">
+      <c r="A39" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B39" t="s">
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="5">
-        <v>45658</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="4">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="18">
+      <c r="A40" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B40" t="s">
         <v>85</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
-      </c>
-      <c r="E40" s="5">
-        <v>45658</v>
+        <v>7</v>
+      </c>
+      <c r="D40" s="4">
+        <v>45717</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1424,17 +1757,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B781A94-BE61-481F-8977-F38608B0EA61}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
@@ -1442,471 +1776,764 @@
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3:B37">_xlfn._xlws.FILTER(Tabela1[[Nome]:[CPF]], (Tabela1[Categoria]="Atleta") + (Tabela1[Categoria]="Associado"), "Lista Vazia")</f>
-        <v>Amanda Santos</v>
-      </c>
-      <c r="B3" s="4" t="str">
-        <v>446.928.320-70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="G3" t="s">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="4" t="str">
-        <v>Ana Guimarães</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>640.535.130-06</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4" t="str">
-        <v>Antonio Gonçalves</v>
-      </c>
-      <c r="B5" s="4" t="str">
-        <v>880.953.950-80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="D23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="4" t="str">
-        <v>Bruna Kiyono</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>635.334.670-07</v>
-      </c>
-      <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="4" t="str">
-        <v>Calebe de Oliveira</v>
-      </c>
-      <c r="B7" s="4" t="str">
-        <v>649.424.580-30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>57</v>
       </c>
-      <c r="G7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="4" t="str">
-        <v>Daniel Hara</v>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v>983.954.920-06</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="4" t="str">
-        <v>Edilson Junior</v>
-      </c>
-      <c r="B9" s="4" t="str">
-        <v>543.590.700-47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="4" t="str">
-        <v>Felipe Soares</v>
-      </c>
-      <c r="B10" s="4" t="str">
-        <v>152.503.150-38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="4" t="str">
-        <v>Gabriel Trigolo</v>
-      </c>
-      <c r="B11" s="4" t="str">
-        <v>790.068.370-40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="4" t="str">
-        <v>Gabriel de Oliveira</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v>341.251.760-78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="4" t="str">
-        <v>Gustavo Ribeiro</v>
-      </c>
-      <c r="B13" s="4" t="str">
-        <v>011.103.590-20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="4" t="str">
-        <v>Heloá Da Silva</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>458.775.990-20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="4" t="str">
-        <v>Heloisa de Oliveira</v>
-      </c>
-      <c r="B15" s="4" t="str">
-        <v>171.537.830-08</v>
-      </c>
-      <c r="C15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="4" t="str">
-        <v>Igor Sena</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>113.551.300-77</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="4" t="str">
-        <v>João Bento</v>
-      </c>
-      <c r="B17" s="4" t="str">
-        <v>738.034.990-20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="4" t="str">
-        <v>João de Almeida</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>848.802.760-57</v>
-      </c>
-      <c r="C18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="4" t="str">
-        <v>João Pinho</v>
-      </c>
-      <c r="B19" s="4" t="str">
-        <v>707.683.290-94</v>
-      </c>
-      <c r="C19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="4" t="str">
-        <v>João Santos</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>501.040.960-71</v>
-      </c>
-      <c r="C20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="4" t="str">
-        <v>Júlia Real</v>
-      </c>
-      <c r="B21" s="4" t="str">
-        <v>905.346.880-39</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q21" t="s">
+      <c r="B36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="4" t="str">
-        <v>Kaue Nunes</v>
-      </c>
-      <c r="B22" s="4" t="str">
-        <v>711.031.530-48</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="4" t="str">
-        <v>Letícia Pereira</v>
-      </c>
-      <c r="B23" s="4" t="str">
-        <v>975.524.820-01</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="4" t="str">
-        <v>Luan Macedo</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <v>454.648.920-01</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="4" t="str">
-        <v>Luanda Vital</v>
-      </c>
-      <c r="B25" s="4" t="str">
-        <v>216.652.530-02</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="4" t="str">
-        <v>Lucas Bruck</v>
-      </c>
-      <c r="B26" s="4" t="str">
-        <v>978.074.480-08</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="4" t="str">
-        <v>Luiz Pinto</v>
-      </c>
-      <c r="B27" s="4" t="str">
-        <v>290.456.840-98</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="4" t="str">
-        <v>Marcelo Ruiz</v>
-      </c>
-      <c r="B28" s="4" t="str">
-        <v>355.157.500-20</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" t="str">
-        <v>Maria Santos</v>
-      </c>
-      <c r="B29" s="4" t="str">
-        <v>352.057.710-03</v>
-      </c>
-      <c r="C29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" t="str">
-        <v>Mateus Pazinatto</v>
-      </c>
-      <c r="B30" t="str">
-        <v>451.727.610-47</v>
-      </c>
-      <c r="C30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" t="str">
-        <v>Matheus Fenili</v>
-      </c>
-      <c r="B31" t="str">
-        <v>102.590.770-11</v>
-      </c>
-      <c r="C31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" t="str">
-        <v>Natalia Massari</v>
-      </c>
-      <c r="B32" t="str">
-        <v>036.678.680-65</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="str">
-        <v>Nestor Junior</v>
-      </c>
-      <c r="B33" t="str">
-        <v>504.682.600-30</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="str">
-        <v>Rhafaela  Oliveira</v>
-      </c>
-      <c r="B34" t="str">
-        <v>666.679.320-09</v>
-      </c>
-      <c r="C34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="str">
-        <v>Yaron Büchler</v>
-      </c>
-      <c r="B35" t="str">
-        <v>591.381.000-70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="str">
-        <v>Matheus Durão</v>
-      </c>
-      <c r="B36" t="str">
-        <v>067.960.780-39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="str">
-        <v>Pedro Oliveira</v>
-      </c>
-      <c r="B37" t="str">
-        <v>145.806.020-99</v>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D0BF37-714A-4C35-9206-0E5BF6C8F7A7}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="10">
+        <v>200</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="I2" t="str" cm="1">
+        <f t="array" ref="I2:I4">_xlfn.UNIQUE(Tabela3[Time], FALSE, FALSE)</f>
+        <v>C2 - Phoenix</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="11">
+        <v>350</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="I3" t="str">
+        <v>C3 - Immortals</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="11">
+        <v>350</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="I4" t="str">
+        <v>AS C2 - Betas</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>